<commit_message>
Update expected test results
</commit_message>
<xml_diff>
--- a/data/test_expected_values.xlsx
+++ b/data/test_expected_values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexs\Dropbox\Dev\f1_fantasy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F452F770-8F42-4196-A86E-091BFE17805C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCFF5DA-CF1A-4808-A569-C46E03E134BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8F73BD9-0904-4916-81F8-0E4EA1678C10}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B8F73BD9-0904-4916-81F8-0E4EA1678C10}"/>
   </bookViews>
   <sheets>
     <sheet name="2003 Expected" sheetId="2" r:id="rId1"/>
@@ -496,11 +496,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E5DE5DB-5BF7-41CE-BB16-C410E9F3C59E}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -812,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" ref="H6:J6" si="3">SUM(G3:G5)</f>
+        <f t="shared" ref="H6" si="3">SUM(G3:G5)</f>
         <v>0</v>
       </c>
       <c r="I6" s="3">
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" ref="H7:J7" si="7">SUM(G4:G6)</f>
+        <f t="shared" ref="H7" si="7">SUM(G4:G6)</f>
         <v>0</v>
       </c>
       <c r="I7" s="3">
@@ -922,7 +922,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" ref="H8:J8" si="9">SUM(G5:G7)</f>
+        <f t="shared" ref="H8" si="9">SUM(G5:G7)</f>
         <v>0</v>
       </c>
       <c r="I8" s="3">
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" ref="H9:J9" si="11">SUM(G6:G8)</f>
+        <f t="shared" ref="H9" si="11">SUM(G6:G8)</f>
         <v>0</v>
       </c>
       <c r="I9" s="3">
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" ref="H10:J10" si="13">SUM(G7:G9)</f>
+        <f t="shared" ref="H10" si="13">SUM(G7:G9)</f>
         <v>0</v>
       </c>
       <c r="I10" s="3">
@@ -1087,7 +1087,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" ref="H11:J11" si="15">SUM(G8:G10)</f>
+        <f t="shared" ref="H11" si="15">SUM(G8:G10)</f>
         <v>0</v>
       </c>
       <c r="I11" s="3">
@@ -1142,7 +1142,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" ref="H12:J12" si="17">SUM(G9:G11)</f>
+        <f t="shared" ref="H12" si="17">SUM(G9:G11)</f>
         <v>0</v>
       </c>
       <c r="I12" s="3">
@@ -1197,7 +1197,7 @@
         <v>7</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" ref="H13:J13" si="19">SUM(G10:G12)</f>
+        <f t="shared" ref="H13" si="19">SUM(G10:G12)</f>
         <v>2</v>
       </c>
       <c r="I13" s="3">
@@ -1208,7 +1208,7 @@
         <v>4.5</v>
       </c>
       <c r="K13" s="3">
-        <f>H13/J13</f>
+        <f t="shared" ref="K2:K22" si="21">H13/J13</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="L13" s="3">
@@ -1256,18 +1256,18 @@
         <v>0</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" ref="H14:J14" si="21">SUM(G11:G13)</f>
+        <f t="shared" ref="H14" si="22">SUM(G11:G13)</f>
         <v>9</v>
       </c>
       <c r="I14" s="3">
         <v>0</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" ref="J14" si="22">SUM(I11:I13)</f>
+        <f t="shared" ref="J14" si="23">SUM(I11:I13)</f>
         <v>9</v>
       </c>
       <c r="K14" s="3">
-        <f>H14/J14</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="L14" s="3">
@@ -1315,18 +1315,18 @@
         <v>0</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" ref="H15:J15" si="23">SUM(G12:G14)</f>
+        <f t="shared" ref="H15" si="24">SUM(G12:G14)</f>
         <v>9</v>
       </c>
       <c r="I15" s="3">
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" ref="J15" si="24">SUM(I12:I14)</f>
+        <f t="shared" ref="J15" si="25">SUM(I12:I14)</f>
         <v>9</v>
       </c>
       <c r="K15" s="3">
-        <f>H15/J15</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="L15" s="3">
@@ -1374,15 +1374,19 @@
         <v>0</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" ref="H16:J16" si="25">SUM(G13:G15)</f>
+        <f t="shared" ref="H16" si="26">SUM(G13:G15)</f>
         <v>7</v>
       </c>
       <c r="I16" s="3">
         <v>0</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" ref="J16" si="26">SUM(I13:I15)</f>
+        <f t="shared" ref="J16" si="27">SUM(I13:I15)</f>
         <v>4.5</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="21"/>
+        <v>1.5555555555555556</v>
       </c>
       <c r="L16" s="3">
         <v>54</v>
@@ -1429,14 +1433,14 @@
         <v>0</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" ref="H17:J17" si="27">SUM(G14:G16)</f>
+        <f t="shared" ref="H17" si="28">SUM(G14:G16)</f>
         <v>0</v>
       </c>
       <c r="I17" s="3">
         <v>0</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" ref="J17" si="28">SUM(I14:I16)</f>
+        <f t="shared" ref="J17" si="29">SUM(I14:I16)</f>
         <v>0</v>
       </c>
       <c r="L17" s="3">
@@ -1484,14 +1488,14 @@
         <v>0</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" ref="H18:J18" si="29">SUM(G15:G17)</f>
+        <f t="shared" ref="H18" si="30">SUM(G15:G17)</f>
         <v>0</v>
       </c>
       <c r="I18" s="3">
         <v>0</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" ref="J18" si="30">SUM(I15:I17)</f>
+        <f t="shared" ref="J18" si="31">SUM(I15:I17)</f>
         <v>0</v>
       </c>
       <c r="L18" s="3">
@@ -1539,14 +1543,14 @@
         <v>1</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" ref="H19:J19" si="31">SUM(G16:G18)</f>
+        <f t="shared" ref="H19" si="32">SUM(G16:G18)</f>
         <v>0</v>
       </c>
       <c r="I19" s="3">
         <v>4.5</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" ref="J19" si="32">SUM(I16:I18)</f>
+        <f t="shared" ref="J19" si="33">SUM(I16:I18)</f>
         <v>0</v>
       </c>
       <c r="L19" s="3">
@@ -1594,18 +1598,18 @@
         <v>12</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" ref="H20:J20" si="33">SUM(G17:G19)</f>
+        <f t="shared" ref="H20" si="34">SUM(G17:G19)</f>
         <v>1</v>
       </c>
       <c r="I20" s="3">
         <v>4.5</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" ref="J20" si="34">SUM(I17:I19)</f>
+        <f t="shared" ref="J20" si="35">SUM(I17:I19)</f>
         <v>4.5</v>
       </c>
       <c r="K20" s="3">
-        <f>H20/J20</f>
+        <f t="shared" si="21"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="L20" s="3">
@@ -1653,18 +1657,18 @@
         <v>10</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" ref="H21:J21" si="35">SUM(G18:G20)</f>
+        <f t="shared" ref="H21" si="36">SUM(G18:G20)</f>
         <v>13</v>
       </c>
       <c r="I21" s="3">
         <v>5</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" ref="J21" si="36">SUM(I18:I20)</f>
+        <f t="shared" ref="J21" si="37">SUM(I18:I20)</f>
         <v>9</v>
       </c>
       <c r="K21" s="3">
-        <f>H21/J21</f>
+        <f t="shared" si="21"/>
         <v>1.4444444444444444</v>
       </c>
       <c r="L21" s="3">
@@ -1712,18 +1716,18 @@
         <v>6</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" ref="H22:J22" si="37">SUM(G19:G21)</f>
+        <f t="shared" ref="H22" si="38">SUM(G19:G21)</f>
         <v>23</v>
       </c>
       <c r="I22" s="3">
         <v>5.5</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" ref="J22" si="38">SUM(I19:I21)</f>
+        <f t="shared" ref="J22" si="39">SUM(I19:I21)</f>
         <v>14</v>
       </c>
       <c r="K22" s="3">
-        <f>H22/J22</f>
+        <f t="shared" si="21"/>
         <v>1.6428571428571428</v>
       </c>
       <c r="L22" s="3">
@@ -1771,14 +1775,14 @@
         <v>11</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" ref="H23:J23" si="39">SUM(G20:G22)</f>
+        <f t="shared" ref="H23" si="40">SUM(G20:G22)</f>
         <v>28</v>
       </c>
       <c r="I23" s="3">
         <v>5.5</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" ref="J23" si="40">SUM(I20:I22)</f>
+        <f t="shared" ref="J23" si="41">SUM(I20:I22)</f>
         <v>15</v>
       </c>
       <c r="K23" s="3">
@@ -2207,11 +2211,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2784D71-4AC0-4629-BA1E-E13CC0397A92}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2303,7 +2307,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F3:F24" si="0">C4/E4</f>
+        <f t="shared" ref="F2:F25" si="0">C4/E4</f>
         <v>1.8571428571428572</v>
       </c>
     </row>
@@ -2338,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" ref="C6:E25" si="1">SUM(B3:B5)</f>
+        <f t="shared" ref="C6:C25" si="1">SUM(B3:B5)</f>
         <v>26</v>
       </c>
       <c r="D6" s="3">
@@ -2348,7 +2352,10 @@
         <f t="shared" ref="E6" si="2">SUM(D3:D5)</f>
         <v>14</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8571428571428572</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3">
@@ -2654,7 +2661,10 @@
         <f t="shared" ref="E21" si="17">SUM(D18:D20)</f>
         <v>15</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="3">
@@ -2740,7 +2750,10 @@
         <f t="shared" ref="E25" si="21">SUM(D22:D24)</f>
         <v>13.3</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="F25" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Driver name encodes constructor, improve handling of mid-season team swaps
</commit_message>
<xml_diff>
--- a/data/test_expected_values.xlsx
+++ b/data/test_expected_values.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCFF5DA-CF1A-4808-A569-C46E03E134BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B8F73BD9-0904-4916-81F8-0E4EA1678C10}"/>
+    <workbookView activeTab="2" windowHeight="15840" windowWidth="29040" xWindow="-120" xr2:uid="{B8F73BD9-0904-4916-81F8-0E4EA1678C10}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="2003 Expected" sheetId="2" r:id="rId1"/>
@@ -117,38 +117,50 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Inter"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <name val="Inter"/>
     </font>
     <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -162,15 +174,25 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -493,8 +515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E5DE5DB-5BF7-41CE-BB16-C410E9F3C59E}">
-  <dimension ref="A1:P23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E5DE5DB-5BF7-41CE-BB16-C410E9F3C59E}">
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -503,7 +524,7 @@
       <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -521,7 +542,7 @@
     <col min="14" max="14" width="13.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="3"/>
+    <col min="17" max="16384" width="9.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="4" customFormat="1">
@@ -579,42 +600,42 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <f t="array" ref="B2:B23">TRANSPOSE('2023 Actual'!C1:X1)</f>
+        <f>TRANSPOSE('2023 Actual'!C1:X1)</f>
         <v>35</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
       </c>
       <c r="D2" s="3">
-        <f t="array" ref="D2:D23">TRANSPOSE('2023 Actual'!C2:X2)</f>
+        <f>TRANSPOSE('2023 Actual'!C2:X2)</f>
         <v>26.9</v>
       </c>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="G2" s="3">
-        <f t="array" ref="G2:G23">TRANSPOSE('2023 Actual'!C3:X3)</f>
+        <f>TRANSPOSE('2023 Actual'!C3:X3)</f>
         <v>0</v>
       </c>
       <c r="H2" s="3">
         <v>0</v>
       </c>
       <c r="I2" s="3">
-        <f t="array" ref="I2:I23">TRANSPOSE('2023 Actual'!C4:X4)</f>
+        <f>TRANSPOSE('2023 Actual'!C4:X4)</f>
         <v>0</v>
       </c>
       <c r="J2" s="3">
         <v>0</v>
       </c>
       <c r="L2" s="3">
-        <f t="array" ref="L2:L23">TRANSPOSE('2023 Actual'!C5:X5)</f>
+        <f>TRANSPOSE('2023 Actual'!C5:X5)</f>
         <v>78</v>
       </c>
       <c r="M2" s="3">
         <v>0</v>
       </c>
       <c r="N2" s="3">
-        <f t="array" ref="N2:N23">TRANSPOSE('2023 Actual'!C6:X6)</f>
+        <f>TRANSPOSE('2023 Actual'!C6:X6)</f>
         <v>27.2</v>
       </c>
       <c r="O2" s="3">
@@ -640,8 +661,8 @@
         <v>26.9</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F23" si="0">C3/E3</f>
-        <v>1.3011152416356877</v>
+        <f>C3/E3</f>
+        <v>1.30111524163569</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -672,8 +693,8 @@
         <v>27.2</v>
       </c>
       <c r="P3" s="3">
-        <f t="shared" ref="P3:P23" si="1">M3/O3</f>
-        <v>2.8676470588235294</v>
+        <f>M3/O3</f>
+        <v>2.86764705882353</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -695,8 +716,8 @@
         <v>53.9</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" si="0"/>
-        <v>1.7810760667903525</v>
+        <f>C4/E4</f>
+        <v>1.78107606679035</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -727,8 +748,8 @@
         <v>54.5</v>
       </c>
       <c r="P4" s="3">
-        <f t="shared" si="1"/>
-        <v>3.1743119266055047</v>
+        <f>M4/O4</f>
+        <v>3.1743119266055</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -750,8 +771,8 @@
         <v>81</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6296296296296295</v>
+        <f>C5/E5</f>
+        <v>1.62962962962963</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -779,11 +800,11 @@
       </c>
       <c r="O5" s="3">
         <f>SUM(N2:N4)</f>
-        <v>81.900000000000006</v>
+        <v>81.9</v>
       </c>
       <c r="P5" s="3">
-        <f t="shared" si="1"/>
-        <v>3.3089133089133087</v>
+        <f>M5/O5</f>
+        <v>3.30891330891331</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -794,51 +815,51 @@
         <v>64</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" ref="C6:E23" si="2">SUM(B3:B5)</f>
+        <f>SUM(B3:B5)</f>
         <v>134</v>
       </c>
       <c r="D6" s="3">
         <v>27.3</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D3:D5)</f>
         <v>81.3</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6482164821648218</v>
+        <f>C6/E6</f>
+        <v>1.64821648216482</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" ref="H6" si="3">SUM(G3:G5)</f>
+        <f>SUM(G3:G5)</f>
         <v>0</v>
       </c>
       <c r="I6" s="3">
         <v>0</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" ref="J6" si="4">SUM(I3:I5)</f>
+        <f>SUM(I3:I5)</f>
         <v>0</v>
       </c>
       <c r="L6" s="3">
         <v>97</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" ref="M6:M23" si="5">SUM(L3:L5)</f>
+        <f>SUM(L3:L5)</f>
         <v>301</v>
       </c>
       <c r="N6" s="3">
         <v>27.6</v>
       </c>
       <c r="O6" s="3">
-        <f t="shared" ref="O6:O23" si="6">SUM(N3:N5)</f>
+        <f>SUM(N3:N5)</f>
         <v>82.2</v>
       </c>
       <c r="P6" s="3">
-        <f t="shared" si="1"/>
-        <v>3.6618004866180049</v>
+        <f>M6/O6</f>
+        <v>3.661800486618</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -849,51 +870,51 @@
         <v>35</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B4:B6)</f>
         <v>137</v>
       </c>
       <c r="D7" s="3">
         <v>27.4</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="2"/>
-        <v>81.599999999999994</v>
+        <f>SUM(D4:D6)</f>
+        <v>81.6</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="0"/>
-        <v>1.678921568627451</v>
+        <f>C7/E7</f>
+        <v>1.67892156862745</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" ref="H7" si="7">SUM(G4:G6)</f>
+        <f>SUM(G4:G6)</f>
         <v>0</v>
       </c>
       <c r="I7" s="3">
         <v>0</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" ref="J7" si="8">SUM(I4:I6)</f>
+        <f>SUM(I4:I6)</f>
         <v>0</v>
       </c>
       <c r="L7" s="3">
         <v>63</v>
       </c>
       <c r="M7" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L4:L6)</f>
         <v>303</v>
       </c>
       <c r="N7" s="3">
         <v>27.7</v>
       </c>
       <c r="O7" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N4:N6)</f>
         <v>82.5</v>
       </c>
       <c r="P7" s="3">
-        <f t="shared" si="1"/>
-        <v>3.6727272727272728</v>
+        <f>M7/O7</f>
+        <v>3.67272727272727</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -904,51 +925,51 @@
         <v>46</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B5:B7)</f>
         <v>136</v>
       </c>
       <c r="D8" s="3">
         <v>27.5</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="2"/>
-        <v>81.900000000000006</v>
+        <f>SUM(D5:D7)</f>
+        <v>81.9</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6605616605616604</v>
+        <f>C8/E8</f>
+        <v>1.66056166056166</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" ref="H8" si="9">SUM(G5:G7)</f>
+        <f>SUM(G5:G7)</f>
         <v>0</v>
       </c>
       <c r="I8" s="3">
         <v>0</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" ref="J8" si="10">SUM(I5:I7)</f>
+        <f>SUM(I5:I7)</f>
         <v>0</v>
       </c>
       <c r="L8" s="3">
         <v>96</v>
       </c>
       <c r="M8" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L5:L7)</f>
         <v>268</v>
       </c>
       <c r="N8" s="3">
         <v>27.8</v>
       </c>
       <c r="O8" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N5:N7)</f>
         <v>82.8</v>
       </c>
       <c r="P8" s="3">
-        <f t="shared" si="1"/>
-        <v>3.2367149758454108</v>
+        <f>M8/O8</f>
+        <v>3.23671497584541</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -959,51 +980,51 @@
         <v>35</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B6:B8)</f>
         <v>145</v>
       </c>
       <c r="D9" s="3">
         <v>27.6</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D6:D8)</f>
         <v>82.2</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="0"/>
-        <v>1.7639902676399026</v>
+        <f>C9/E9</f>
+        <v>1.7639902676399</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" ref="H9" si="11">SUM(G6:G8)</f>
+        <f>SUM(G6:G8)</f>
         <v>0</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" ref="J9" si="12">SUM(I6:I8)</f>
+        <f>SUM(I6:I8)</f>
         <v>0</v>
       </c>
       <c r="L9" s="3">
         <v>86</v>
       </c>
       <c r="M9" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L6:L8)</f>
         <v>256</v>
       </c>
       <c r="N9" s="3">
         <v>27.9</v>
       </c>
       <c r="O9" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N6:N8)</f>
         <v>83.1</v>
       </c>
       <c r="P9" s="3">
-        <f t="shared" si="1"/>
-        <v>3.0806257521058966</v>
+        <f>M9/O9</f>
+        <v>3.0806257521059</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1014,51 +1035,51 @@
         <v>56</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B7:B9)</f>
         <v>116</v>
       </c>
       <c r="D10" s="3">
         <v>27.8</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D7:D9)</f>
         <v>82.5</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="0"/>
-        <v>1.406060606060606</v>
+        <f>C10/E10</f>
+        <v>1.40606060606061</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" ref="H10" si="13">SUM(G7:G9)</f>
+        <f>SUM(G7:G9)</f>
         <v>0</v>
       </c>
       <c r="I10" s="3">
         <v>0</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" ref="J10" si="14">SUM(I7:I9)</f>
+        <f>SUM(I7:I9)</f>
         <v>0</v>
       </c>
       <c r="L10" s="3">
         <v>112</v>
       </c>
       <c r="M10" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L7:L9)</f>
         <v>245</v>
       </c>
       <c r="N10" s="3">
         <v>28.1</v>
       </c>
       <c r="O10" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N7:N9)</f>
         <v>83.4</v>
       </c>
       <c r="P10" s="3">
-        <f t="shared" si="1"/>
-        <v>2.9376498800959232</v>
+        <f>M10/O10</f>
+        <v>2.93764988009592</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1069,51 +1090,51 @@
         <v>46</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B8:B10)</f>
         <v>137</v>
       </c>
       <c r="D11" s="3">
         <v>27.9</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D8:D10)</f>
         <v>82.9</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="0"/>
-        <v>1.6525934861278648</v>
+        <f>C11/E11</f>
+        <v>1.65259348612786</v>
       </c>
       <c r="G11" s="3">
         <v>0</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" ref="H11" si="15">SUM(G8:G10)</f>
+        <f>SUM(G8:G10)</f>
         <v>0</v>
       </c>
       <c r="I11" s="3">
         <v>0</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" ref="J11" si="16">SUM(I8:I10)</f>
+        <f>SUM(I8:I10)</f>
         <v>0</v>
       </c>
       <c r="L11" s="3">
         <v>77</v>
       </c>
       <c r="M11" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L8:L10)</f>
         <v>294</v>
       </c>
       <c r="N11" s="3">
         <v>28.2</v>
       </c>
       <c r="O11" s="3">
-        <f t="shared" si="6"/>
-        <v>83.800000000000011</v>
+        <f>SUM(N8:N10)</f>
+        <v>83.8</v>
       </c>
       <c r="P11" s="3">
-        <f t="shared" si="1"/>
-        <v>3.5083532219570399</v>
+        <f>M11/O11</f>
+        <v>3.50835322195704</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1124,51 +1145,51 @@
         <v>46</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B9:B11)</f>
         <v>137</v>
       </c>
       <c r="D12" s="3">
         <v>28.1</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="2"/>
-        <v>83.300000000000011</v>
+        <f>SUM(D9:D11)</f>
+        <v>83.3</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="0"/>
-        <v>1.644657863145258</v>
+        <f>C12/E12</f>
+        <v>1.64465786314526</v>
       </c>
       <c r="G12" s="3">
         <v>2</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" ref="H12" si="17">SUM(G9:G11)</f>
+        <f>SUM(G9:G11)</f>
         <v>0</v>
       </c>
       <c r="I12" s="3">
         <v>4.5</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" ref="J12" si="18">SUM(I9:I11)</f>
+        <f>SUM(I9:I11)</f>
         <v>0</v>
       </c>
       <c r="L12" s="3">
         <v>95</v>
       </c>
       <c r="M12" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L9:L11)</f>
         <v>275</v>
       </c>
       <c r="N12" s="3">
         <v>28.4</v>
       </c>
       <c r="O12" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N9:N11)</f>
         <v>84.2</v>
       </c>
       <c r="P12" s="3">
-        <f t="shared" si="1"/>
-        <v>3.2660332541567696</v>
+        <f>M12/O12</f>
+        <v>3.26603325415677</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1179,55 +1200,55 @@
         <v>68</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B10:B12)</f>
         <v>148</v>
       </c>
       <c r="D13" s="3">
         <v>28.3</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="2"/>
-        <v>83.800000000000011</v>
+        <f>SUM(D10:D12)</f>
+        <v>83.8</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="0"/>
-        <v>1.7661097852028638</v>
+        <f>C13/E13</f>
+        <v>1.76610978520286</v>
       </c>
       <c r="G13" s="3">
         <v>7</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" ref="H13" si="19">SUM(G10:G12)</f>
+        <f>SUM(G10:G12)</f>
         <v>2</v>
       </c>
       <c r="I13" s="3">
         <v>4.5</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" ref="J13" si="20">SUM(I10:I12)</f>
+        <f>SUM(I10:I12)</f>
         <v>4.5</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" ref="K2:K22" si="21">H13/J13</f>
-        <v>0.44444444444444442</v>
+        <f>H13/J13</f>
+        <v>0.444444444444444</v>
       </c>
       <c r="L13" s="3">
         <v>80</v>
       </c>
       <c r="M13" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L10:L12)</f>
         <v>284</v>
       </c>
       <c r="N13" s="3">
         <v>28.6</v>
       </c>
       <c r="O13" s="3">
-        <f t="shared" si="6"/>
-        <v>84.699999999999989</v>
+        <f>SUM(N10:N12)</f>
+        <v>84.7</v>
       </c>
       <c r="P13" s="3">
-        <f t="shared" si="1"/>
-        <v>3.3530106257378991</v>
+        <f>M13/O13</f>
+        <v>3.3530106257379</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1238,55 +1259,55 @@
         <v>46</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B11:B13)</f>
         <v>160</v>
       </c>
       <c r="D14" s="3">
         <v>28.5</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D11:D13)</f>
         <v>84.3</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="0"/>
-        <v>1.8979833926453145</v>
+        <f>C14/E14</f>
+        <v>1.89798339264531</v>
       </c>
       <c r="G14" s="3">
         <v>0</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" ref="H14" si="22">SUM(G11:G13)</f>
+        <f>SUM(G11:G13)</f>
         <v>9</v>
       </c>
       <c r="I14" s="3">
         <v>0</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" ref="J14" si="23">SUM(I11:I13)</f>
+        <f>SUM(I11:I13)</f>
         <v>9</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" si="21"/>
+        <f>H14/J14</f>
         <v>1</v>
       </c>
       <c r="L14" s="3">
         <v>101</v>
       </c>
       <c r="M14" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L11:L13)</f>
         <v>252</v>
       </c>
       <c r="N14" s="3">
         <v>28.7</v>
       </c>
       <c r="O14" s="3">
-        <f t="shared" si="6"/>
-        <v>85.199999999999989</v>
+        <f>SUM(N11:N13)</f>
+        <v>85.2</v>
       </c>
       <c r="P14" s="3">
-        <f t="shared" si="1"/>
-        <v>2.9577464788732399</v>
+        <f>M14/O14</f>
+        <v>2.95774647887324</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1297,55 +1318,55 @@
         <v>38</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B12:B14)</f>
         <v>160</v>
       </c>
       <c r="D15" s="3">
         <v>28.6</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D12:D14)</f>
         <v>84.9</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="0"/>
-        <v>1.884570082449941</v>
+        <f>C15/E15</f>
+        <v>1.88457008244994</v>
       </c>
       <c r="G15" s="3">
         <v>0</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" ref="H15" si="24">SUM(G12:G14)</f>
+        <f>SUM(G12:G14)</f>
         <v>9</v>
       </c>
       <c r="I15" s="3">
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" ref="J15" si="25">SUM(I12:I14)</f>
+        <f>SUM(I12:I14)</f>
         <v>9</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" si="21"/>
+        <f>H15/J15</f>
         <v>1</v>
       </c>
       <c r="L15" s="3">
         <v>81</v>
       </c>
       <c r="M15" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L12:L14)</f>
         <v>276</v>
       </c>
       <c r="N15" s="3">
         <v>28.8</v>
       </c>
       <c r="O15" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N12:N14)</f>
         <v>85.7</v>
       </c>
       <c r="P15" s="3">
-        <f t="shared" si="1"/>
-        <v>3.220536756126021</v>
+        <f>M15/O15</f>
+        <v>3.22053675612602</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1356,55 +1377,55 @@
         <v>25</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B13:B15)</f>
         <v>152</v>
       </c>
       <c r="D16" s="3">
         <v>28.8</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D13:D15)</f>
         <v>85.4</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="0"/>
-        <v>1.7798594847775175</v>
+        <f>C16/E16</f>
+        <v>1.77985948477752</v>
       </c>
       <c r="G16" s="3">
         <v>0</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" ref="H16" si="26">SUM(G13:G15)</f>
+        <f>SUM(G13:G15)</f>
         <v>7</v>
       </c>
       <c r="I16" s="3">
         <v>0</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" ref="J16" si="27">SUM(I13:I15)</f>
+        <f>SUM(I13:I15)</f>
         <v>4.5</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="21"/>
-        <v>1.5555555555555556</v>
+        <f>H16/J16</f>
+        <v>1.55555555555556</v>
       </c>
       <c r="L16" s="3">
         <v>54</v>
       </c>
       <c r="M16" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L13:L15)</f>
         <v>262</v>
       </c>
       <c r="N16" s="3">
         <v>29</v>
       </c>
       <c r="O16" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N13:N15)</f>
         <v>86.1</v>
       </c>
       <c r="P16" s="3">
-        <f t="shared" si="1"/>
-        <v>3.0429732868757262</v>
+        <f>M16/O16</f>
+        <v>3.04297328687573</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1415,51 +1436,51 @@
         <v>47</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B14:B16)</f>
         <v>109</v>
       </c>
       <c r="D17" s="3">
         <v>28.9</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D14:D16)</f>
         <v>85.9</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="0"/>
-        <v>1.2689173457508731</v>
+        <f>C17/E17</f>
+        <v>1.26891734575087</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" ref="H17" si="28">SUM(G14:G16)</f>
+        <f>SUM(G14:G16)</f>
         <v>0</v>
       </c>
       <c r="I17" s="3">
         <v>0</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" ref="J17" si="29">SUM(I14:I16)</f>
+        <f>SUM(I14:I16)</f>
         <v>0</v>
       </c>
       <c r="L17" s="3">
         <v>46</v>
       </c>
       <c r="M17" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L14:L16)</f>
         <v>236</v>
       </c>
       <c r="N17" s="3">
         <v>29.1</v>
       </c>
       <c r="O17" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N14:N16)</f>
         <v>86.5</v>
       </c>
       <c r="P17" s="3">
-        <f t="shared" si="1"/>
-        <v>2.7283236994219653</v>
+        <f>M17/O17</f>
+        <v>2.72832369942197</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1470,51 +1491,51 @@
         <v>62</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B15:B17)</f>
         <v>110</v>
       </c>
       <c r="D18" s="3">
         <v>29.1</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="2"/>
-        <v>86.300000000000011</v>
+        <f>SUM(D15:D17)</f>
+        <v>86.3</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="0"/>
-        <v>1.2746234067207414</v>
+        <f>C18/E18</f>
+        <v>1.27462340672074</v>
       </c>
       <c r="G18" s="3">
         <v>0</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" ref="H18" si="30">SUM(G15:G17)</f>
+        <f>SUM(G15:G17)</f>
         <v>0</v>
       </c>
       <c r="I18" s="3">
         <v>0</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" ref="J18" si="31">SUM(I15:I17)</f>
+        <f>SUM(I15:I17)</f>
         <v>0</v>
       </c>
       <c r="L18" s="3">
         <v>64</v>
       </c>
       <c r="M18" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L15:L17)</f>
         <v>181</v>
       </c>
       <c r="N18" s="3">
         <v>29.2</v>
       </c>
       <c r="O18" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N15:N17)</f>
         <v>86.9</v>
       </c>
       <c r="P18" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0828538550057538</v>
+        <f>M18/O18</f>
+        <v>2.08285385500575</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1525,51 +1546,51 @@
         <v>53</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B16:B18)</f>
         <v>134</v>
       </c>
       <c r="D19" s="3">
         <v>29.3</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="2"/>
-        <v>86.800000000000011</v>
+        <f>SUM(D16:D18)</f>
+        <v>86.8</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="0"/>
-        <v>1.5437788018433178</v>
+        <f>C19/E19</f>
+        <v>1.54377880184332</v>
       </c>
       <c r="G19" s="3">
         <v>1</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" ref="H19" si="32">SUM(G16:G18)</f>
+        <f>SUM(G16:G18)</f>
         <v>0</v>
       </c>
       <c r="I19" s="3">
         <v>4.5</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" ref="J19" si="33">SUM(I16:I18)</f>
+        <f>SUM(I16:I18)</f>
         <v>0</v>
       </c>
       <c r="L19" s="3">
         <v>95</v>
       </c>
       <c r="M19" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L16:L18)</f>
         <v>164</v>
       </c>
       <c r="N19" s="3">
         <v>29.3</v>
       </c>
       <c r="O19" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N16:N18)</f>
         <v>87.3</v>
       </c>
       <c r="P19" s="3">
-        <f t="shared" si="1"/>
-        <v>1.8785796105383734</v>
+        <f>M19/O19</f>
+        <v>1.87857961053837</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1580,55 +1601,55 @@
         <v>42</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B17:B19)</f>
         <v>162</v>
       </c>
       <c r="D20" s="3">
         <v>29.5</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D17:D19)</f>
         <v>87.3</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="0"/>
-        <v>1.8556701030927836</v>
+        <f>C20/E20</f>
+        <v>1.85567010309278</v>
       </c>
       <c r="G20" s="3">
         <v>12</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" ref="H20" si="34">SUM(G17:G19)</f>
+        <f>SUM(G17:G19)</f>
         <v>1</v>
       </c>
       <c r="I20" s="3">
         <v>4.5</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" ref="J20" si="35">SUM(I17:I19)</f>
+        <f>SUM(I17:I19)</f>
         <v>4.5</v>
       </c>
       <c r="K20" s="3">
-        <f t="shared" si="21"/>
-        <v>0.22222222222222221</v>
+        <f>H20/J20</f>
+        <v>0.222222222222222</v>
       </c>
       <c r="L20" s="3">
         <v>45</v>
       </c>
       <c r="M20" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L17:L19)</f>
         <v>205</v>
       </c>
       <c r="N20" s="3">
         <v>29.4</v>
       </c>
       <c r="O20" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N17:N19)</f>
         <v>87.6</v>
       </c>
       <c r="P20" s="3">
-        <f t="shared" si="1"/>
-        <v>2.3401826484018264</v>
+        <f>M20/O20</f>
+        <v>2.34018264840183</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1639,55 +1660,55 @@
         <v>45</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B18:B20)</f>
         <v>157</v>
       </c>
       <c r="D21" s="3">
         <v>29.7</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D18:D20)</f>
         <v>87.9</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="0"/>
-        <v>1.7861205915813423</v>
+        <f>C21/E21</f>
+        <v>1.78612059158134</v>
       </c>
       <c r="G21" s="3">
         <v>10</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" ref="H21" si="36">SUM(G18:G20)</f>
+        <f>SUM(G18:G20)</f>
         <v>13</v>
       </c>
       <c r="I21" s="3">
         <v>5</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" ref="J21" si="37">SUM(I18:I20)</f>
+        <f>SUM(I18:I20)</f>
         <v>9</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="21"/>
-        <v>1.4444444444444444</v>
+        <f>H21/J21</f>
+        <v>1.44444444444444</v>
       </c>
       <c r="L21" s="3">
         <v>105</v>
       </c>
       <c r="M21" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L18:L20)</f>
         <v>204</v>
       </c>
       <c r="N21" s="3">
         <v>29.4</v>
       </c>
       <c r="O21" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N18:N20)</f>
         <v>87.9</v>
       </c>
       <c r="P21" s="3">
-        <f t="shared" si="1"/>
-        <v>2.3208191126279862</v>
+        <f>M21/O21</f>
+        <v>2.32081911262799</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1698,55 +1719,55 @@
         <v>44</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B19:B21)</f>
         <v>140</v>
       </c>
       <c r="D22" s="3">
         <v>29.9</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D19:D21)</f>
         <v>88.5</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="0"/>
-        <v>1.5819209039548023</v>
+        <f>C22/E22</f>
+        <v>1.5819209039548</v>
       </c>
       <c r="G22" s="3">
         <v>6</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" ref="H22" si="38">SUM(G19:G21)</f>
+        <f>SUM(G19:G21)</f>
         <v>23</v>
       </c>
       <c r="I22" s="3">
         <v>5.5</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" ref="J22" si="39">SUM(I19:I21)</f>
+        <f>SUM(I19:I21)</f>
         <v>14</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" si="21"/>
-        <v>1.6428571428571428</v>
+        <f>H22/J22</f>
+        <v>1.64285714285714</v>
       </c>
       <c r="L22" s="3">
         <v>84</v>
       </c>
       <c r="M22" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L19:L21)</f>
         <v>245</v>
       </c>
       <c r="N22" s="3">
         <v>29.6</v>
       </c>
       <c r="O22" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N19:N21)</f>
         <v>88.1</v>
       </c>
       <c r="P22" s="3">
-        <f t="shared" si="1"/>
-        <v>2.7809307604994324</v>
+        <f>M22/O22</f>
+        <v>2.78093076049943</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1757,55 +1778,55 @@
         <v>47</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B20:B22)</f>
         <v>131</v>
       </c>
       <c r="D23" s="3">
         <v>30</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(D20:D22)</f>
         <v>89.1</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>1.4702581369248038</v>
+        <f>C23/E23</f>
+        <v>1.4702581369248</v>
       </c>
       <c r="G23" s="3">
         <v>11</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" ref="H23" si="40">SUM(G20:G22)</f>
+        <f>SUM(G20:G22)</f>
         <v>28</v>
       </c>
       <c r="I23" s="3">
         <v>5.5</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" ref="J23" si="41">SUM(I20:I22)</f>
+        <f>SUM(I20:I22)</f>
         <v>15</v>
       </c>
       <c r="K23" s="3">
         <f>H23/J23</f>
-        <v>1.8666666666666667</v>
+        <v>1.86666666666667</v>
       </c>
       <c r="L23" s="3">
         <v>87</v>
       </c>
       <c r="M23" s="3">
-        <f t="shared" si="5"/>
+        <f>SUM(L20:L22)</f>
         <v>234</v>
       </c>
       <c r="N23" s="3">
         <v>29.7</v>
       </c>
       <c r="O23" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(N20:N22)</f>
         <v>88.4</v>
       </c>
       <c r="P23" s="3">
-        <f t="shared" si="1"/>
-        <v>2.6470588235294117</v>
+        <f>M23/O23</f>
+        <v>2.64705882352941</v>
       </c>
     </row>
   </sheetData>
@@ -1815,14 +1836,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1F4C22-B1F0-4432-9D5D-AC861A522885}">
-  <dimension ref="A1:X6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1F4C22-B1F0-4432-9D5D-AC861A522885}">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:24" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
@@ -2208,17 +2228,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2784D71-4AC0-4629-BA1E-E13CC0397A92}">
-  <dimension ref="A1:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2784D71-4AC0-4629-BA1E-E13CC0397A92}">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0" tabSelected="1">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -2253,14 +2272,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <f t="array" ref="B2:B25">TRANSPOSE('2004 Actual'!C3:Z3)</f>
+        <f>TRANSPOSE('2004 Actual'!C3:Z3)</f>
         <v>0</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
       </c>
       <c r="D2" s="3">
-        <f t="array" ref="D2:D25">TRANSPOSE('2004 Actual'!C6:Z6)</f>
+        <f>TRANSPOSE('2004 Actual'!C6:Z6)</f>
         <v>0</v>
       </c>
       <c r="E2" s="3">
@@ -2273,7 +2292,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3">
         <f>B2</f>
@@ -2297,7 +2316,7 @@
       </c>
       <c r="C4" s="3">
         <f>SUM(B2:B3)</f>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -2306,10 +2325,7 @@
         <f>SUM(D2:D3)</f>
         <v>14</v>
       </c>
-      <c r="F4" s="3">
-        <f t="shared" ref="F2:F25" si="0">C4/E4</f>
-        <v>1.8571428571428572</v>
-      </c>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3">
@@ -2320,7 +2336,7 @@
       </c>
       <c r="C5" s="3">
         <f>SUM(B2:B4)</f>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -2329,10 +2345,7 @@
         <f>SUM(D2:D4)</f>
         <v>14</v>
       </c>
-      <c r="F5" s="3">
-        <f t="shared" si="0"/>
-        <v>1.8571428571428572</v>
-      </c>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3">
@@ -2342,20 +2355,17 @@
         <v>0</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" ref="C6:C25" si="1">SUM(B3:B5)</f>
-        <v>26</v>
+        <f>SUM(B3:B5)</f>
+        <v>0</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" ref="E6" si="2">SUM(D3:D5)</f>
+        <f>SUM(D3:D5)</f>
         <v>14</v>
       </c>
-      <c r="F6" s="3">
-        <f t="shared" si="0"/>
-        <v>1.8571428571428572</v>
-      </c>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3">
@@ -2365,14 +2375,14 @@
         <v>0</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B4:B6)</f>
         <v>0</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ref="E7" si="3">SUM(D4:D6)</f>
+        <f>SUM(D4:D6)</f>
         <v>0</v>
       </c>
       <c r="F7" s="3"/>
@@ -2385,14 +2395,14 @@
         <v>0</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B5:B7)</f>
         <v>0</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" ref="E8" si="4">SUM(D5:D7)</f>
+        <f>SUM(D5:D7)</f>
         <v>0</v>
       </c>
       <c r="F8" s="3"/>
@@ -2405,14 +2415,14 @@
         <v>0</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B6:B8)</f>
         <v>0</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" ref="E9" si="5">SUM(D6:D8)</f>
+        <f>SUM(D6:D8)</f>
         <v>0</v>
       </c>
       <c r="F9" s="3"/>
@@ -2425,14 +2435,14 @@
         <v>0</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B7:B9)</f>
         <v>0</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" ref="E10" si="6">SUM(D7:D9)</f>
+        <f>SUM(D7:D9)</f>
         <v>0</v>
       </c>
       <c r="F10" s="3"/>
@@ -2445,14 +2455,14 @@
         <v>0</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B8:B10)</f>
         <v>0</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" ref="E11" si="7">SUM(D8:D10)</f>
+        <f>SUM(D8:D10)</f>
         <v>0</v>
       </c>
       <c r="F11" s="3"/>
@@ -2465,14 +2475,14 @@
         <v>0</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B9:B11)</f>
         <v>0</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" ref="E12" si="8">SUM(D9:D11)</f>
+        <f>SUM(D9:D11)</f>
         <v>0</v>
       </c>
       <c r="F12" s="3"/>
@@ -2485,14 +2495,14 @@
         <v>0</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B10:B12)</f>
         <v>0</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" ref="E13" si="9">SUM(D10:D12)</f>
+        <f>SUM(D10:D12)</f>
         <v>0</v>
       </c>
       <c r="F13" s="3"/>
@@ -2505,14 +2515,14 @@
         <v>0</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B11:B13)</f>
         <v>0</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" ref="E14" si="10">SUM(D11:D13)</f>
+        <f>SUM(D11:D13)</f>
         <v>0</v>
       </c>
       <c r="F14" s="3"/>
@@ -2525,14 +2535,14 @@
         <v>0</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B12:B14)</f>
         <v>0</v>
       </c>
       <c r="D15" s="3">
         <v>0</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" ref="E15" si="11">SUM(D12:D14)</f>
+        <f>SUM(D12:D14)</f>
         <v>0</v>
       </c>
       <c r="F15" s="3"/>
@@ -2545,14 +2555,14 @@
         <v>0</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B13:B15)</f>
         <v>0</v>
       </c>
       <c r="D16" s="3">
         <v>0</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" ref="E16" si="12">SUM(D13:D15)</f>
+        <f>SUM(D13:D15)</f>
         <v>0</v>
       </c>
       <c r="F16" s="3"/>
@@ -2565,14 +2575,14 @@
         <v>0</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B14:B16)</f>
         <v>0</v>
       </c>
       <c r="D17" s="3">
         <v>0</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" ref="E17" si="13">SUM(D14:D16)</f>
+        <f>SUM(D14:D16)</f>
         <v>0</v>
       </c>
       <c r="F17" s="3"/>
@@ -2585,14 +2595,14 @@
         <v>7</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B15:B17)</f>
         <v>0</v>
       </c>
       <c r="D18" s="3">
         <v>15</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" ref="E18" si="14">SUM(D15:D17)</f>
+        <f>SUM(D15:D17)</f>
         <v>0</v>
       </c>
       <c r="F18" s="3"/>
@@ -2605,19 +2615,19 @@
         <v>0</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B16:B18)</f>
         <v>7</v>
       </c>
       <c r="D19" s="3">
         <v>0</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" ref="E19" si="15">SUM(D16:D18)</f>
+        <f>SUM(D16:D18)</f>
         <v>15</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+        <f>C19/E19</f>
+        <v>0.466666666666667</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2628,19 +2638,19 @@
         <v>0</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B17:B19)</f>
         <v>7</v>
       </c>
       <c r="D20" s="3">
         <v>0</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" ref="E20" si="16">SUM(D17:D19)</f>
+        <f>SUM(D17:D19)</f>
         <v>15</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+        <f>C20/E20</f>
+        <v>0.466666666666667</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2651,19 +2661,19 @@
         <v>0</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B18:B20)</f>
         <v>7</v>
       </c>
       <c r="D21" s="3">
         <v>0</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" ref="E21" si="17">SUM(D18:D20)</f>
+        <f>SUM(D18:D20)</f>
         <v>15</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+        <f>C21/E21</f>
+        <v>0.466666666666667</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2674,14 +2684,14 @@
         <v>14</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B19:B21)</f>
         <v>0</v>
       </c>
       <c r="D22" s="3">
         <v>13.3</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" ref="E22" si="18">SUM(D19:D21)</f>
+        <f>SUM(D19:D21)</f>
         <v>0</v>
       </c>
       <c r="F22" s="3"/>
@@ -2694,19 +2704,19 @@
         <v>0</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B20:B22)</f>
         <v>14</v>
       </c>
       <c r="D23" s="3">
         <v>0</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" ref="E23" si="19">SUM(D20:D22)</f>
+        <f>SUM(D20:D22)</f>
         <v>13.3</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>1.0526315789473684</v>
+        <f>C23/E23</f>
+        <v>1.05263157894737</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2717,19 +2727,19 @@
         <v>0</v>
       </c>
       <c r="C24" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B21:B23)</f>
         <v>14</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" ref="E24" si="20">SUM(D21:D23)</f>
+        <f>SUM(D21:D23)</f>
         <v>13.3</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="0"/>
-        <v>1.0526315789473684</v>
+        <f>C24/E24</f>
+        <v>1.05263157894737</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2740,19 +2750,19 @@
         <v>0</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="1"/>
+        <f>SUM(B22:B24)</f>
         <v>14</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" ref="E25" si="21">SUM(D22:D24)</f>
+        <f>SUM(D22:D24)</f>
         <v>13.3</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="0"/>
-        <v>1.0526315789473684</v>
+        <f>C25/E25</f>
+        <v>1.05263157894737</v>
       </c>
     </row>
   </sheetData>
@@ -2761,14 +2771,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91EF152-550E-48F4-9F27-F94F2D7CA7F7}">
-  <dimension ref="A1:Z6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91EF152-550E-48F4-9F27-F94F2D7CA7F7}">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection pane="topLeft" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
@@ -2844,100 +2853,100 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <f>C1+C2</f>
         <v>0</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:W3" si="0">D1+D2</f>
+      <c r="D3" s="1">
+        <f>D1+D2</f>
         <v>26</v>
       </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <f t="shared" si="0"/>
+      <c r="E3" s="0">
+        <f>E1+E2</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="0">
+        <f>F1+F2</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="0">
+        <f>G1+G2</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="0">
+        <f>H1+H2</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="0">
+        <f>I1+I2</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="0">
+        <f>J1+J2</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="0">
+        <f>K1+K2</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="0">
+        <f>L1+L2</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="0">
+        <f>M1+M2</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="0">
+        <f>N1+N2</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="0">
+        <f>O1+O2</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="0">
+        <f>P1+P2</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="0">
+        <f>Q1+Q2</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="0">
+        <f>R1+R2</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <f>S1+S2</f>
         <v>7</v>
       </c>
-      <c r="T3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <f t="shared" si="0"/>
+      <c r="T3" s="0">
+        <f>T1+T2</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="0">
+        <f>U1+U2</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="0">
+        <f>V1+V2</f>
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
+        <f>W1+W2</f>
         <v>14</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="0">
         <f>X1+X2</f>
         <v>0</v>
       </c>
-      <c r="Y3">
-        <f t="shared" ref="Y3" si="1">Y1+Y2</f>
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <f t="shared" ref="Z3" si="2">Z1+Z2</f>
+      <c r="Y3" s="0">
+        <f>Y1+Y2</f>
+        <v>0</v>
+      </c>
+      <c r="Z3" s="0">
+        <f>Z1+Z2</f>
         <v>0</v>
       </c>
     </row>
@@ -3015,100 +3024,100 @@
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <f>SUM(C4:C5)</f>
         <v>0</v>
       </c>
-      <c r="D6">
-        <f t="shared" ref="D6:Z6" si="3">SUM(D4:D5)</f>
+      <c r="D6" s="0">
+        <f>SUM(D4:D5)</f>
         <v>14</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="3"/>
+      <c r="E6" s="0">
+        <f>SUM(E4:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="0">
+        <f>SUM(F4:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="0">
+        <f>SUM(G4:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="0">
+        <f>SUM(H4:H5)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="0">
+        <f>SUM(I4:I5)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="0">
+        <f>SUM(J4:J5)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="0">
+        <f>SUM(K4:K5)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="0">
+        <f>SUM(L4:L5)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="0">
+        <f>SUM(M4:M5)</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="0">
+        <f>SUM(N4:N5)</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="0">
+        <f>SUM(O4:O5)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="0">
+        <f>SUM(P4:P5)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="0">
+        <f>SUM(Q4:Q5)</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="0">
+        <f>SUM(R4:R5)</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="0">
+        <f>SUM(S4:S5)</f>
         <v>15</v>
       </c>
-      <c r="T6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <f t="shared" si="3"/>
+      <c r="T6" s="0">
+        <f>SUM(T4:T5)</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="0">
+        <f>SUM(U4:U5)</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="0">
+        <f>SUM(V4:V5)</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="0">
+        <f>SUM(W4:W5)</f>
         <v>13.3</v>
       </c>
-      <c r="X6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" si="3"/>
+      <c r="X6" s="0">
+        <f>SUM(X4:X5)</f>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="0">
+        <f>SUM(Y4:Y5)</f>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="0">
+        <f>SUM(Z4:Z5)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>